<commit_message>
Updated commit ABDM project
</commit_message>
<xml_diff>
--- a/src/main/java/Configuration/XPath&TestData.xlsx
+++ b/src/main/java/Configuration/XPath&TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\ABDM_Automation_Script.v.2\src\main\java\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\ABDM_Automation_Script.v.20\src\main\java\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04E1901-01A1-4548-8DEF-FBB48798F2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810B06D5-6C83-4113-B4E2-2D65F443E8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{58B16572-EE6B-45BA-A1E3-D73DD5D73692}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>WebElement Name</t>
   </si>
@@ -178,9 +178,6 @@
     <t>Healthcare1122@gmail</t>
   </si>
   <si>
-    <t>Healthcare@1</t>
-  </si>
-  <si>
     <t>screenShotPath</t>
   </si>
   <si>
@@ -244,7 +241,7 @@
     <t>C:\\\\Users\\\\USER\\\\eclipse-workspace\\\\ABDM_Automation_Script\\\\EXTENT_REPORT</t>
   </si>
   <si>
-    <t>C:\\Users\\USER\\eclipse-workspace\\ABDM_Automation_Script.v.2\\ScreenShots\\</t>
+    <t>C:\\Users\\USER\\eclipse-workspace\\ABDM_Automation_Script.v.20\\ScreenShots\\</t>
   </si>
 </sst>
 </file>
@@ -685,31 +682,28 @@
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D8344D1E-A31D-4385-B3B8-671A54C896BB}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{DF34ECBB-A566-4037-80B7-B53CAE4FFE6E}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{FBBF580F-8B82-4C63-91ED-6546232246C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -739,18 +733,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -788,7 +782,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -796,7 +790,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -804,7 +798,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -812,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -820,7 +814,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -828,7 +822,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -836,7 +830,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
@@ -844,7 +838,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -852,7 +846,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -860,7 +854,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -868,7 +862,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -876,7 +870,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -884,7 +878,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -892,7 +886,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -905,7 +899,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B13"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>